<commit_message>
Solved problems with nodekinds
</commit_message>
<xml_diff>
--- a/diagrams/TableNodeKind.xlsx
+++ b/diagrams/TableNodeKind.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\salgo\Developer\tesis\shacl_integration\diagrams\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D32BFB29-B748-45DA-A853-50DF9F2891EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{483AFB25-4480-4F5B-A958-C5860E3D8A50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="20832" windowHeight="16656" activeTab="1" xr2:uid="{B07788D2-E141-4477-B793-2407B8167394}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" xr2:uid="{B07788D2-E141-4477-B793-2407B8167394}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="160">
   <si>
     <t>IRI</t>
   </si>
@@ -514,6 +514,9 @@
   </si>
   <si>
     <t>OPERATION TYPE</t>
+  </si>
+  <si>
+    <t>IRIOrLiteral, BlankNodeOrIRI</t>
   </si>
 </sst>
 </file>
@@ -1411,11 +1414,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06BE7C6B-FC15-41EF-81DC-0E014A9BDF86}">
-  <dimension ref="A1:J53"/>
+  <dimension ref="A1:J82"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A45" sqref="A45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I71" sqref="I71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2739,7 +2742,786 @@
       <c r="H52" s="34"/>
       <c r="I52" s="25"/>
     </row>
-    <row r="53" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="53" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B53" s="1">
+        <v>1</v>
+      </c>
+      <c r="C53" s="1">
+        <v>0</v>
+      </c>
+      <c r="D53" s="1">
+        <v>0</v>
+      </c>
+      <c r="E53" s="1">
+        <v>1</v>
+      </c>
+      <c r="F53" s="1">
+        <v>0</v>
+      </c>
+      <c r="G53" s="1">
+        <v>1</v>
+      </c>
+      <c r="H53" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A54" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B54" s="1">
+        <v>1</v>
+      </c>
+      <c r="C54" s="1">
+        <v>0</v>
+      </c>
+      <c r="D54" s="1">
+        <v>0</v>
+      </c>
+      <c r="E54" s="1">
+        <v>1</v>
+      </c>
+      <c r="F54" s="1">
+        <v>1</v>
+      </c>
+      <c r="G54" s="1">
+        <v>0</v>
+      </c>
+      <c r="H54" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A55" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B55" s="1">
+        <v>1</v>
+      </c>
+      <c r="C55" s="1">
+        <v>0</v>
+      </c>
+      <c r="D55" s="1">
+        <v>0</v>
+      </c>
+      <c r="E55" s="1">
+        <v>0</v>
+      </c>
+      <c r="F55" s="1">
+        <v>1</v>
+      </c>
+      <c r="G55" s="1">
+        <v>1</v>
+      </c>
+      <c r="H55" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A56" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B56" s="1">
+        <v>1</v>
+      </c>
+      <c r="C56" s="1">
+        <v>0</v>
+      </c>
+      <c r="D56" s="1">
+        <v>0</v>
+      </c>
+      <c r="E56" s="1">
+        <v>1</v>
+      </c>
+      <c r="F56" s="1">
+        <v>1</v>
+      </c>
+      <c r="G56" s="1">
+        <v>1</v>
+      </c>
+      <c r="H56" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A57" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B57" s="1">
+        <v>0</v>
+      </c>
+      <c r="C57" s="1">
+        <v>1</v>
+      </c>
+      <c r="D57" s="1">
+        <v>0</v>
+      </c>
+      <c r="E57" s="1">
+        <v>1</v>
+      </c>
+      <c r="F57" s="1">
+        <v>0</v>
+      </c>
+      <c r="G57" s="1">
+        <v>1</v>
+      </c>
+      <c r="H57" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A58" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B58" s="1">
+        <v>0</v>
+      </c>
+      <c r="C58" s="1">
+        <v>1</v>
+      </c>
+      <c r="D58" s="1">
+        <v>0</v>
+      </c>
+      <c r="E58" s="1">
+        <v>1</v>
+      </c>
+      <c r="F58" s="1">
+        <v>1</v>
+      </c>
+      <c r="G58" s="1">
+        <v>0</v>
+      </c>
+      <c r="H58" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A59" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B59" s="1">
+        <v>0</v>
+      </c>
+      <c r="C59" s="1">
+        <v>1</v>
+      </c>
+      <c r="D59" s="1">
+        <v>0</v>
+      </c>
+      <c r="E59" s="1">
+        <v>0</v>
+      </c>
+      <c r="F59" s="1">
+        <v>1</v>
+      </c>
+      <c r="G59" s="1">
+        <v>1</v>
+      </c>
+      <c r="H59" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A60" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B60" s="1">
+        <v>0</v>
+      </c>
+      <c r="C60" s="1">
+        <v>1</v>
+      </c>
+      <c r="D60" s="1">
+        <v>0</v>
+      </c>
+      <c r="E60" s="1">
+        <v>1</v>
+      </c>
+      <c r="F60" s="1">
+        <v>1</v>
+      </c>
+      <c r="G60" s="1">
+        <v>1</v>
+      </c>
+      <c r="H60" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A61" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B61" s="1">
+        <v>0</v>
+      </c>
+      <c r="C61" s="1">
+        <v>0</v>
+      </c>
+      <c r="D61" s="1">
+        <v>1</v>
+      </c>
+      <c r="E61" s="1">
+        <v>1</v>
+      </c>
+      <c r="F61" s="1">
+        <v>0</v>
+      </c>
+      <c r="G61" s="1">
+        <v>1</v>
+      </c>
+      <c r="H61" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A62" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B62" s="1">
+        <v>0</v>
+      </c>
+      <c r="C62" s="1">
+        <v>0</v>
+      </c>
+      <c r="D62" s="1">
+        <v>1</v>
+      </c>
+      <c r="E62" s="1">
+        <v>1</v>
+      </c>
+      <c r="F62" s="1">
+        <v>1</v>
+      </c>
+      <c r="G62" s="1">
+        <v>0</v>
+      </c>
+      <c r="H62" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A63" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B63" s="1">
+        <v>0</v>
+      </c>
+      <c r="C63" s="1">
+        <v>0</v>
+      </c>
+      <c r="D63" s="1">
+        <v>1</v>
+      </c>
+      <c r="E63" s="1">
+        <v>0</v>
+      </c>
+      <c r="F63" s="1">
+        <v>1</v>
+      </c>
+      <c r="G63" s="1">
+        <v>1</v>
+      </c>
+      <c r="H63" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A64" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B64" s="1">
+        <v>0</v>
+      </c>
+      <c r="C64" s="1">
+        <v>0</v>
+      </c>
+      <c r="D64" s="1">
+        <v>1</v>
+      </c>
+      <c r="E64" s="1">
+        <v>1</v>
+      </c>
+      <c r="F64" s="1">
+        <v>1</v>
+      </c>
+      <c r="G64" s="1">
+        <v>1</v>
+      </c>
+      <c r="H64" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A65" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B65" s="1">
+        <v>0</v>
+      </c>
+      <c r="C65" s="1">
+        <v>0</v>
+      </c>
+      <c r="D65" s="1">
+        <v>0</v>
+      </c>
+      <c r="E65" s="1">
+        <v>1</v>
+      </c>
+      <c r="F65" s="1">
+        <v>0</v>
+      </c>
+      <c r="G65" s="1">
+        <v>1</v>
+      </c>
+      <c r="H65" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A66" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B66" s="1">
+        <v>0</v>
+      </c>
+      <c r="C66" s="1">
+        <v>0</v>
+      </c>
+      <c r="D66" s="1">
+        <v>0</v>
+      </c>
+      <c r="E66" s="1">
+        <v>1</v>
+      </c>
+      <c r="F66" s="1">
+        <v>1</v>
+      </c>
+      <c r="G66" s="1">
+        <v>0</v>
+      </c>
+      <c r="H66" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A67" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B67" s="1">
+        <v>0</v>
+      </c>
+      <c r="C67" s="1">
+        <v>0</v>
+      </c>
+      <c r="D67" s="1">
+        <v>0</v>
+      </c>
+      <c r="E67" s="1">
+        <v>0</v>
+      </c>
+      <c r="F67" s="1">
+        <v>1</v>
+      </c>
+      <c r="G67" s="1">
+        <v>1</v>
+      </c>
+      <c r="H67" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A68" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B68" s="1">
+        <v>0</v>
+      </c>
+      <c r="C68" s="1">
+        <v>0</v>
+      </c>
+      <c r="D68" s="1">
+        <v>0</v>
+      </c>
+      <c r="E68" s="1">
+        <v>1</v>
+      </c>
+      <c r="F68" s="1">
+        <v>1</v>
+      </c>
+      <c r="G68" s="1">
+        <v>1</v>
+      </c>
+      <c r="H68" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A69" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B69" s="1">
+        <v>1</v>
+      </c>
+      <c r="C69" s="1">
+        <v>1</v>
+      </c>
+      <c r="D69" s="1">
+        <v>1</v>
+      </c>
+      <c r="E69" s="1">
+        <v>0</v>
+      </c>
+      <c r="F69" s="1">
+        <v>0</v>
+      </c>
+      <c r="G69" s="1">
+        <v>0</v>
+      </c>
+      <c r="H69" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A70" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B70" s="1">
+        <v>1</v>
+      </c>
+      <c r="C70" s="1">
+        <v>1</v>
+      </c>
+      <c r="D70" s="1">
+        <v>0</v>
+      </c>
+      <c r="E70" s="1">
+        <v>1</v>
+      </c>
+      <c r="F70" s="1">
+        <v>0</v>
+      </c>
+      <c r="G70" s="1">
+        <v>1</v>
+      </c>
+      <c r="H70" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A71" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B71" s="1">
+        <v>1</v>
+      </c>
+      <c r="C71" s="1">
+        <v>1</v>
+      </c>
+      <c r="D71" s="1">
+        <v>0</v>
+      </c>
+      <c r="E71" s="1">
+        <v>1</v>
+      </c>
+      <c r="F71" s="1">
+        <v>1</v>
+      </c>
+      <c r="G71" s="1">
+        <v>0</v>
+      </c>
+      <c r="H71" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A72" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B72" s="1">
+        <v>1</v>
+      </c>
+      <c r="C72" s="1">
+        <v>1</v>
+      </c>
+      <c r="D72" s="1">
+        <v>0</v>
+      </c>
+      <c r="E72" s="1">
+        <v>0</v>
+      </c>
+      <c r="F72" s="1">
+        <v>1</v>
+      </c>
+      <c r="G72" s="1">
+        <v>1</v>
+      </c>
+      <c r="H72" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A73" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B73" s="1">
+        <v>1</v>
+      </c>
+      <c r="C73" s="1">
+        <v>1</v>
+      </c>
+      <c r="D73" s="1">
+        <v>0</v>
+      </c>
+      <c r="E73" s="1">
+        <v>1</v>
+      </c>
+      <c r="F73" s="1">
+        <v>1</v>
+      </c>
+      <c r="G73" s="1">
+        <v>1</v>
+      </c>
+      <c r="H73" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A74" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B74" s="1">
+        <v>1</v>
+      </c>
+      <c r="C74" s="1">
+        <v>0</v>
+      </c>
+      <c r="D74" s="1">
+        <v>1</v>
+      </c>
+      <c r="E74" s="1">
+        <v>1</v>
+      </c>
+      <c r="F74" s="1">
+        <v>0</v>
+      </c>
+      <c r="G74" s="1">
+        <v>1</v>
+      </c>
+      <c r="H74" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A75" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B75" s="1">
+        <v>1</v>
+      </c>
+      <c r="C75" s="1">
+        <v>0</v>
+      </c>
+      <c r="D75" s="1">
+        <v>1</v>
+      </c>
+      <c r="E75" s="1">
+        <v>1</v>
+      </c>
+      <c r="F75" s="1">
+        <v>1</v>
+      </c>
+      <c r="G75" s="1">
+        <v>0</v>
+      </c>
+      <c r="H75" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A76" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B76" s="1">
+        <v>1</v>
+      </c>
+      <c r="C76" s="1">
+        <v>0</v>
+      </c>
+      <c r="D76" s="1">
+        <v>1</v>
+      </c>
+      <c r="E76" s="1">
+        <v>0</v>
+      </c>
+      <c r="F76" s="1">
+        <v>1</v>
+      </c>
+      <c r="G76" s="1">
+        <v>1</v>
+      </c>
+      <c r="H76" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A77" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B77" s="1">
+        <v>1</v>
+      </c>
+      <c r="C77" s="1">
+        <v>0</v>
+      </c>
+      <c r="D77" s="1">
+        <v>1</v>
+      </c>
+      <c r="E77" s="1">
+        <v>1</v>
+      </c>
+      <c r="F77" s="1">
+        <v>1</v>
+      </c>
+      <c r="G77" s="1">
+        <v>1</v>
+      </c>
+      <c r="H77" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A78" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B78" s="1">
+        <v>0</v>
+      </c>
+      <c r="C78" s="1">
+        <v>1</v>
+      </c>
+      <c r="D78" s="1">
+        <v>1</v>
+      </c>
+      <c r="E78" s="1">
+        <v>1</v>
+      </c>
+      <c r="F78" s="1">
+        <v>0</v>
+      </c>
+      <c r="G78" s="1">
+        <v>1</v>
+      </c>
+      <c r="H78" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A79" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B79" s="1">
+        <v>0</v>
+      </c>
+      <c r="C79" s="1">
+        <v>1</v>
+      </c>
+      <c r="D79" s="1">
+        <v>1</v>
+      </c>
+      <c r="E79" s="1">
+        <v>1</v>
+      </c>
+      <c r="F79" s="1">
+        <v>1</v>
+      </c>
+      <c r="G79" s="1">
+        <v>0</v>
+      </c>
+      <c r="H79" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A80" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B80" s="1">
+        <v>0</v>
+      </c>
+      <c r="C80" s="1">
+        <v>1</v>
+      </c>
+      <c r="D80" s="1">
+        <v>1</v>
+      </c>
+      <c r="E80" s="1">
+        <v>0</v>
+      </c>
+      <c r="F80" s="1">
+        <v>1</v>
+      </c>
+      <c r="G80" s="1">
+        <v>1</v>
+      </c>
+      <c r="H80" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A81" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B81" s="1">
+        <v>0</v>
+      </c>
+      <c r="C81" s="1">
+        <v>1</v>
+      </c>
+      <c r="D81" s="1">
+        <v>1</v>
+      </c>
+      <c r="E81" s="1">
+        <v>1</v>
+      </c>
+      <c r="F81" s="1">
+        <v>1</v>
+      </c>
+      <c r="G81" s="1">
+        <v>1</v>
+      </c>
+      <c r="H81" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A82" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B82" s="1">
+        <v>1</v>
+      </c>
+      <c r="C82" s="1">
+        <v>1</v>
+      </c>
+      <c r="D82" s="1">
+        <v>1</v>
+      </c>
+      <c r="E82" s="1">
+        <v>1</v>
+      </c>
+      <c r="F82" s="1">
+        <v>1</v>
+      </c>
+      <c r="G82" s="1">
+        <v>1</v>
+      </c>
+      <c r="H82" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="A17:H17"/>
@@ -2756,11 +3538,14 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FCEA4B1-0F42-4530-8705-691EA53A091E}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:I55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J6" sqref="J6"/>
+      <selection pane="bottomLeft" activeCell="H2" sqref="H2:I55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4373,6 +5158,7 @@
     </row>
   </sheetData>
   <phoneticPr fontId="9" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="76" fitToHeight="0" orientation="landscape" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>